<commit_message>
added local docs as backup
</commit_message>
<xml_diff>
--- a/docs/datasets/coins_comparison.xlsx
+++ b/docs/datasets/coins_comparison.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marvinottersberg/Documents/GitHub/sentiment-trading/docs/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marvinottersberg/Documents/GitHub/sentiment/docs/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79FF1E3-2177-DA4A-9F26-D69E17135DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D558274D-CAD4-B54B-A103-F465C4ECE204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{0FBE6ABC-E7BC-FF47-8F89-7CBAE8928606}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{0FBE6ABC-E7BC-FF47-8F89-7CBAE8928606}"/>
   </bookViews>
   <sheets>
     <sheet name="Coinmarketcap_532022" sheetId="1" r:id="rId1"/>
     <sheet name="Social Media Relevance_14032022" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,9 +122,6 @@
     <t>37.327 (as of 2021)</t>
   </si>
   <si>
-    <t>Total Circulating Supply (in million)</t>
-  </si>
-  <si>
     <t>18,975 BTC</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Reddit Members (in million)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Circulating Supply </t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -240,7 +240,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADFA78A-DD24-3D45-B508-FAB576027403}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,22 +684,22 @@
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -820,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B0209D-A63F-6A40-A4DB-542E2E00408D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +856,7 @@
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3">
         <v>4.8</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>2330</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>

</xml_diff>